<commit_message>
Update excel file format
</commit_message>
<xml_diff>
--- a/output/account_bpmb_20180601.xlsx
+++ b/output/account_bpmb_20180601.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Main_acc" sheetId="3" r:id="rId1"/>
     <sheet name="CHILD_FORM" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Users" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
   <si>
     <t>STT</t>
   </si>
@@ -123,28 +124,52 @@
     <t>Child form</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>dainv_1</t>
-  </si>
-  <si>
-    <t>dainv_2</t>
-  </si>
-  <si>
-    <t>dainv_3</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>tw_admins</t>
+  </si>
+  <si>
+    <t>tw_managers</t>
+  </si>
+  <si>
+    <t>appInstName</t>
+  </si>
+  <si>
+    <t>BPMBService</t>
+  </si>
+  <si>
+    <t>dainv1_1</t>
+  </si>
+  <si>
+    <t>dainv1_2</t>
+  </si>
+  <si>
+    <t>dainv1_3</t>
+  </si>
+  <si>
+    <t>dainv1_4</t>
+  </si>
+  <si>
+    <t>dainv1_5</t>
+  </si>
+  <si>
+    <t>dainv1_1@gmail.com</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -542,10 +567,16 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -577,12 +608,10 @@
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -599,27 +628,25 @@
         <v>21</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>"dainv_"&amp;A3&amp;"@gmail.com"</f>
-        <v>dainv_1@gmail.com</v>
+        <f>"dainv1_"&amp;A3&amp;"@gmail.com"</f>
+        <v>dainv1_1@gmail.com</v>
       </c>
       <c r="F3" s="1" t="str">
         <f>B3&amp;C3&amp;D3</f>
         <v>A1FK</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>"dainv_"&amp;A3</f>
-        <v>dainv_1</v>
+        <f>"dainv1_"&amp;A3</f>
+        <v>dainv1_1</v>
       </c>
       <c r="H3" s="1" t="str">
         <f>"Hpt123456_"&amp;A3</f>
         <v>Hpt123456_1</v>
       </c>
-      <c r="I3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="I3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -636,23 +663,23 @@
         <v>22</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f t="shared" ref="E4:E11" si="1">"dainv_"&amp;A4&amp;"@gmail.com"</f>
-        <v>dainv_2@gmail.com</v>
+        <f t="shared" ref="E4:E11" si="1">"dainv1_"&amp;A4&amp;"@gmail.com"</f>
+        <v>dainv1_2@gmail.com</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" ref="F4:F11" si="2">B4&amp;C4&amp;D4</f>
         <v>V1GL</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f t="shared" ref="G4:G11" si="3">"dainv_"&amp;A4</f>
-        <v>dainv_2</v>
+        <f t="shared" ref="G4:G11" si="3">"dainv1_"&amp;A4</f>
+        <v>dainv1_2</v>
       </c>
       <c r="H4" s="1" t="str">
         <f t="shared" ref="H4:H11" si="4">"Hpt123456_"&amp;A4</f>
         <v>Hpt123456_2</v>
       </c>
-      <c r="I4" s="1" t="b">
-        <v>0</v>
+      <c r="I4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -672,7 +699,7 @@
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dainv_3@gmail.com</v>
+        <v>dainv1_3@gmail.com</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="2"/>
@@ -680,14 +707,14 @@
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>dainv_3</v>
+        <v>dainv1_3</v>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Hpt123456_3</v>
       </c>
-      <c r="I5" s="1" t="b">
-        <v>0</v>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -707,7 +734,7 @@
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dainv_4@gmail.com</v>
+        <v>dainv1_4@gmail.com</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="2"/>
@@ -715,14 +742,14 @@
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>dainv_4</v>
+        <v>dainv1_4</v>
       </c>
       <c r="H6" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Hpt123456_4</v>
       </c>
-      <c r="I6" s="1" t="b">
-        <v>0</v>
+      <c r="I6" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -742,7 +769,7 @@
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dainv_5@gmail.com</v>
+        <v>dainv1_5@gmail.com</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="2"/>
@@ -750,302 +777,20 @@
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>dainv_5</v>
+        <v>dainv1_5</v>
       </c>
       <c r="H7" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Hpt123456_5</v>
       </c>
-      <c r="I7" s="1" t="b">
-        <v>0</v>
+      <c r="I7" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dainv_6@gmail.com</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>BCD</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>dainv_6</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Hpt123456_6</v>
-      </c>
-      <c r="I8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dainv_7@gmail.com</v>
-      </c>
-      <c r="F9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>EFG</v>
-      </c>
-      <c r="G9" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>dainv_7</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Hpt123456_7</v>
-      </c>
-      <c r="I9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dainv_8@gmail.com</v>
-      </c>
-      <c r="F10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>IIJ</v>
-      </c>
-      <c r="G10" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>dainv_8</v>
-      </c>
-      <c r="H10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Hpt123456_8</v>
-      </c>
-      <c r="I10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dainv_9@gmail.com</v>
-      </c>
-      <c r="F11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>KLM</v>
-      </c>
-      <c r="G11" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>dainv_9</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Hpt123456_9</v>
-      </c>
-      <c r="I11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <f>ROW()-2</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <f t="shared" ref="A4:A11" si="0">ROW()-2</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1056,13 +801,8 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1073,13 +813,8 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1090,13 +825,8 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1111,12 +841,491 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <f>ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A11" si="0">ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <f>ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>"dainv1_"&amp;A3&amp;"@gmail.com"</f>
+        <v>dainv1_1@gmail.com</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>B3&amp;C3&amp;D3</f>
+        <v>dainv1_123</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <f>"dainv1_"&amp;A3</f>
+        <v>dainv1_1</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>"Hpt123456"</f>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A11" si="0">ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4:E11" si="1">"dainv1_"&amp;A4&amp;"@gmail.com"</f>
+        <v>dainv1_2@gmail.com</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" ref="I4:I11" si="2">B4&amp;C4&amp;D4</f>
+        <v>dainv1_223</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f t="shared" ref="J4:J11" si="3">"dainv1_"&amp;A4</f>
+        <v>dainv1_2</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" ref="K4:K7" si="4">"Hpt123456"</f>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv1_3@gmail.com</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dainv1_323</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>dainv1_3</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv1_4@gmail.com</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dainv1_423</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>dainv1_4</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv1_5@gmail.com</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dainv1_523</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>dainv1_5</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update excel files + script
</commit_message>
<xml_diff>
--- a/output/account_bpmb_20180601.xlsx
+++ b/output/account_bpmb_20180601.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Main_acc" sheetId="3" r:id="rId1"/>
     <sheet name="CHILD_FORM" sheetId="4" r:id="rId2"/>
     <sheet name="Users" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Disable" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
   <si>
     <t>STT</t>
   </si>
@@ -157,19 +158,28 @@
     <t>dainv1_5</t>
   </si>
   <si>
-    <t>dainv1_1@gmail.com</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>dainv0_0</t>
+  </si>
+  <si>
+    <t>dainv0_1</t>
+  </si>
+  <si>
+    <t>dainv0_2</t>
+  </si>
+  <si>
+    <t>dainv0_3</t>
+  </si>
+  <si>
+    <t>dainv0_4</t>
+  </si>
+  <si>
+    <t>dainv0_5</t>
   </si>
 </sst>
 </file>
@@ -255,11 +265,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +578,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +661,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A11" si="0">ROW()-2</f>
+        <f t="shared" ref="A4:A7" si="0">ROW()-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -663,19 +674,19 @@
         <v>22</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f t="shared" ref="E4:E11" si="1">"dainv1_"&amp;A4&amp;"@gmail.com"</f>
+        <f t="shared" ref="E4:E7" si="1">"dainv1_"&amp;A4&amp;"@gmail.com"</f>
         <v>dainv1_2@gmail.com</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f t="shared" ref="F4:F11" si="2">B4&amp;C4&amp;D4</f>
+        <f t="shared" ref="F4:F7" si="2">B4&amp;C4&amp;D4</f>
         <v>V1GL</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f t="shared" ref="G4:G11" si="3">"dainv1_"&amp;A4</f>
+        <f t="shared" ref="G4:G7" si="3">"dainv1_"&amp;A4</f>
         <v>dainv1_2</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" ref="H4:H11" si="4">"Hpt123456_"&amp;A4</f>
+        <f t="shared" ref="H4:H7" si="4">"Hpt123456_"&amp;A4</f>
         <v>Hpt123456_2</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -884,7 +895,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A11" si="0">ROW()-2</f>
+        <f t="shared" ref="A4:A6" si="0">ROW()-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -966,14 +977,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1072,7 +1091,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A11" si="0">ROW()-2</f>
+        <f t="shared" ref="A4:A7" si="0">ROW()-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1085,7 +1104,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f t="shared" ref="E4:E11" si="1">"dainv1_"&amp;A4&amp;"@gmail.com"</f>
+        <f t="shared" ref="E4:E7" si="1">"dainv1_"&amp;A4&amp;"@gmail.com"</f>
         <v>dainv1_2@gmail.com</v>
       </c>
       <c r="F4" s="1"/>
@@ -1096,11 +1115,11 @@
         <v>4</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f t="shared" ref="I4:I11" si="2">B4&amp;C4&amp;D4</f>
+        <f t="shared" ref="I4:I7" si="2">B4&amp;C4&amp;D4</f>
         <v>dainv1_223</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f t="shared" ref="J4:J11" si="3">"dainv1_"&amp;A4</f>
+        <f t="shared" ref="J4:J7" si="3">"dainv1_"&amp;A4</f>
         <v>dainv1_2</v>
       </c>
       <c r="K4" s="1" t="str">
@@ -1778,4 +1797,360 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <f>ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>"dainv0_"&amp;A3-1&amp;"@gmail.com"</f>
+        <v>dainv0_0@gmail.com</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>B3&amp;C3&amp;D3</f>
+        <v>dainv0_023</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <f>"DAINV0_"&amp;A3-1</f>
+        <v>DAINV0_0</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>"Hpt123456"</f>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A8" si="0">ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4:E8" si="1">"dainv0_"&amp;A4-1&amp;"@gmail.com"</f>
+        <v>dainv0_1@gmail.com</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" ref="I4:I7" si="2">B4&amp;C4&amp;D4</f>
+        <v>dainv0_123</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f t="shared" ref="J4:J8" si="3">"DAINV0_"&amp;A4-1</f>
+        <v>DAINV0_1</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" ref="K4:K8" si="4">"Hpt123456"</f>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv0_2@gmail.com</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dainv0_223</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DAINV0_2</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv0_3@gmail.com</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dainv0_323</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DAINV0_3</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv0_4@gmail.com</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dainv0_423</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DAINV0_4</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dainv0_5@gmail.com</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" ref="I8" si="5">B8&amp;C8&amp;D8</f>
+        <v>dainv0_523</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DAINV0_5</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Hpt123456</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>